<commit_message>
fix for clinician since pt1 not working
</commit_message>
<xml_diff>
--- a/resources/Clinician.xlsx
+++ b/resources/Clinician.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="28695" windowHeight="13290" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="17190" windowHeight="3345" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Clinician" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="338">
   <si>
     <t>Name</t>
   </si>
@@ -442,9 +442,6 @@
     <t>rd</t>
   </si>
   <si>
-    <t>st</t>
-  </si>
-  <si>
     <t>rn</t>
   </si>
   <si>
@@ -1031,6 +1028,15 @@
   </si>
   <si>
     <t>//p[contains(text(),"Aide Care Plan")]</t>
+  </si>
+  <si>
+    <t>pt</t>
+  </si>
+  <si>
+    <t>error notice</t>
+  </si>
+  <si>
+    <t>Unable to view patient on clinician to do visit</t>
   </si>
 </sst>
 </file>
@@ -1401,7 +1407,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="15"/>
@@ -1583,7 +1589,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>24</v>
@@ -1729,7 +1735,7 @@
         <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
@@ -1750,10 +1756,10 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
@@ -1764,10 +1770,10 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
@@ -1798,10 +1804,10 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>77</v>
@@ -1809,7 +1815,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="B7" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>77</v>
@@ -1817,7 +1823,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="B8" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>77</v>
@@ -1825,7 +1831,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>77</v>
@@ -1833,7 +1839,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="B10" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>77</v>
@@ -1841,7 +1847,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="B11" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>77</v>
@@ -1869,10 +1875,10 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>77</v>
@@ -1880,7 +1886,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="B14" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>77</v>
@@ -1888,7 +1894,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="B15" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>77</v>
@@ -1896,7 +1902,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="B16" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>77</v>
@@ -1904,7 +1910,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="B17" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>77</v>
@@ -1912,7 +1918,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="B18" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>77</v>
@@ -1920,7 +1926,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="B19" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>77</v>
@@ -1928,7 +1934,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="B20" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>77</v>
@@ -1936,7 +1942,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="B21" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>77</v>
@@ -1944,7 +1950,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="B22" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>77</v>
@@ -1952,7 +1958,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="B23" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>77</v>
@@ -1960,7 +1966,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="B24" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>77</v>
@@ -1971,13 +1977,13 @@
     </row>
     <row r="25" spans="1:7">
       <c r="B25" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -2002,10 +2008,10 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>12</v>
@@ -2022,7 +2028,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="B28" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>12</v>
@@ -2039,7 +2045,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="B29" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>12</v>
@@ -2056,7 +2062,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="B30" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>12</v>
@@ -2073,7 +2079,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="B31" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>12</v>
@@ -2090,7 +2096,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="B32" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>12</v>
@@ -2107,7 +2113,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="B33" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>12</v>
@@ -2124,7 +2130,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="B34" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>12</v>
@@ -2141,7 +2147,7 @@
     </row>
     <row r="35" spans="1:7">
       <c r="B35" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>12</v>
@@ -2158,7 +2164,7 @@
     </row>
     <row r="36" spans="1:7">
       <c r="B36" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>12</v>
@@ -2175,7 +2181,7 @@
     </row>
     <row r="37" spans="1:7">
       <c r="B37" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>12</v>
@@ -2192,7 +2198,7 @@
     </row>
     <row r="38" spans="1:7">
       <c r="B38" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>12</v>
@@ -2209,7 +2215,7 @@
     </row>
     <row r="39" spans="1:7">
       <c r="B39" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>12</v>
@@ -2226,7 +2232,7 @@
     </row>
     <row r="40" spans="1:7">
       <c r="B40" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>12</v>
@@ -2243,7 +2249,7 @@
     </row>
     <row r="41" spans="1:7">
       <c r="B41" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>12</v>
@@ -2260,7 +2266,7 @@
     </row>
     <row r="42" spans="1:7">
       <c r="B42" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>12</v>
@@ -2277,7 +2283,7 @@
     </row>
     <row r="43" spans="1:7">
       <c r="B43" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>12</v>
@@ -2314,10 +2320,10 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>12</v>
@@ -2334,7 +2340,7 @@
     </row>
     <row r="46" spans="1:7">
       <c r="B46" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>12</v>
@@ -2351,7 +2357,7 @@
     </row>
     <row r="47" spans="1:7" ht="30">
       <c r="B47" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>12</v>
@@ -2368,7 +2374,7 @@
     </row>
     <row r="48" spans="1:7">
       <c r="B48" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>12</v>
@@ -2385,7 +2391,7 @@
     </row>
     <row r="49" spans="1:7" ht="30">
       <c r="B49" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>12</v>
@@ -2402,7 +2408,7 @@
     </row>
     <row r="50" spans="1:7">
       <c r="B50" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>12</v>
@@ -2419,10 +2425,10 @@
     </row>
     <row r="51" spans="1:7" ht="30">
       <c r="A51" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>12</v>
@@ -2439,10 +2445,10 @@
     </row>
     <row r="52" spans="1:7" ht="45">
       <c r="A52" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>12</v>
@@ -2459,10 +2465,10 @@
     </row>
     <row r="53" spans="1:7" ht="30">
       <c r="A53" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>12</v>
@@ -2479,10 +2485,10 @@
     </row>
     <row r="54" spans="1:7" ht="45">
       <c r="A54" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>12</v>
@@ -2499,10 +2505,10 @@
     </row>
     <row r="55" spans="1:7" ht="30">
       <c r="A55" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>260</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>12</v>
@@ -2519,10 +2525,10 @@
     </row>
     <row r="56" spans="1:7" ht="45">
       <c r="A56" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>12</v>
@@ -2539,7 +2545,7 @@
     </row>
     <row r="57" spans="1:7" ht="45">
       <c r="B57" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>12</v>
@@ -2556,7 +2562,7 @@
     </row>
     <row r="58" spans="1:7" ht="45">
       <c r="B58" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>12</v>
@@ -2573,7 +2579,7 @@
     </row>
     <row r="59" spans="1:7">
       <c r="B59" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>12</v>
@@ -2590,7 +2596,7 @@
     </row>
     <row r="60" spans="1:7">
       <c r="B60" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>12</v>
@@ -2607,7 +2613,7 @@
     </row>
     <row r="61" spans="1:7" ht="30">
       <c r="B61" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>77</v>
@@ -2624,7 +2630,7 @@
     </row>
     <row r="62" spans="1:7" ht="30">
       <c r="B62" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>77</v>
@@ -2641,7 +2647,7 @@
     </row>
     <row r="63" spans="1:7" ht="30">
       <c r="B63" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>77</v>
@@ -2658,13 +2664,13 @@
     </row>
     <row r="64" spans="1:7" ht="30">
       <c r="B64" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C64" s="12" t="s">
         <v>33</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E64" s="1">
         <v>1</v>
@@ -2678,10 +2684,10 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>12</v>
@@ -2698,10 +2704,10 @@
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>12</v>
@@ -2718,7 +2724,7 @@
     </row>
     <row r="67" spans="1:7">
       <c r="B67" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>12</v>
@@ -2735,7 +2741,7 @@
     </row>
     <row r="68" spans="1:7" ht="30">
       <c r="B68" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>12</v>
@@ -2752,7 +2758,7 @@
     </row>
     <row r="69" spans="1:7">
       <c r="B69" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>12</v>
@@ -2769,7 +2775,7 @@
     </row>
     <row r="70" spans="1:7" ht="30">
       <c r="B70" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>12</v>
@@ -2786,7 +2792,7 @@
     </row>
     <row r="71" spans="1:7">
       <c r="B71" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>12</v>
@@ -2803,10 +2809,10 @@
     </row>
     <row r="72" spans="1:7" ht="30">
       <c r="A72" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>12</v>
@@ -2823,10 +2829,10 @@
     </row>
     <row r="73" spans="1:7" ht="45">
       <c r="A73" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>12</v>
@@ -2843,10 +2849,10 @@
     </row>
     <row r="74" spans="1:7" ht="30">
       <c r="A74" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>12</v>
@@ -2863,10 +2869,10 @@
     </row>
     <row r="75" spans="1:7" ht="45">
       <c r="A75" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>12</v>
@@ -2883,10 +2889,10 @@
     </row>
     <row r="76" spans="1:7" ht="30">
       <c r="A76" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>12</v>
@@ -2903,10 +2909,10 @@
     </row>
     <row r="77" spans="1:7" ht="45">
       <c r="A77" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>12</v>
@@ -2923,7 +2929,7 @@
     </row>
     <row r="78" spans="1:7" ht="45">
       <c r="B78" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>12</v>
@@ -2940,7 +2946,7 @@
     </row>
     <row r="79" spans="1:7" ht="45">
       <c r="B79" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>12</v>
@@ -2957,7 +2963,7 @@
     </row>
     <row r="80" spans="1:7">
       <c r="B80" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>12</v>
@@ -2974,7 +2980,7 @@
     </row>
     <row r="81" spans="1:7">
       <c r="B81" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>12</v>
@@ -2991,10 +2997,10 @@
     </row>
     <row r="82" spans="1:7">
       <c r="A82" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>12</v>
@@ -3011,10 +3017,10 @@
     </row>
     <row r="83" spans="1:7">
       <c r="A83" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>12</v>
@@ -3031,7 +3037,7 @@
     </row>
     <row r="84" spans="1:7">
       <c r="B84" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>12</v>
@@ -3048,7 +3054,7 @@
     </row>
     <row r="85" spans="1:7" ht="30">
       <c r="B85" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>12</v>
@@ -3065,7 +3071,7 @@
     </row>
     <row r="86" spans="1:7">
       <c r="B86" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>12</v>
@@ -3082,7 +3088,7 @@
     </row>
     <row r="87" spans="1:7" ht="30">
       <c r="B87" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>12</v>
@@ -3099,7 +3105,7 @@
     </row>
     <row r="88" spans="1:7">
       <c r="B88" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>12</v>
@@ -3116,10 +3122,10 @@
     </row>
     <row r="89" spans="1:7" ht="30">
       <c r="A89" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>12</v>
@@ -3136,10 +3142,10 @@
     </row>
     <row r="90" spans="1:7" ht="45">
       <c r="A90" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>12</v>
@@ -3156,10 +3162,10 @@
     </row>
     <row r="91" spans="1:7" ht="30">
       <c r="A91" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>12</v>
@@ -3176,10 +3182,10 @@
     </row>
     <row r="92" spans="1:7" ht="45">
       <c r="A92" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>12</v>
@@ -3196,10 +3202,10 @@
     </row>
     <row r="93" spans="1:7" ht="30">
       <c r="A93" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>12</v>
@@ -3216,10 +3222,10 @@
     </row>
     <row r="94" spans="1:7" ht="45">
       <c r="A94" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>12</v>
@@ -3236,7 +3242,7 @@
     </row>
     <row r="95" spans="1:7" ht="45">
       <c r="B95" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>12</v>
@@ -3253,7 +3259,7 @@
     </row>
     <row r="96" spans="1:7" ht="45">
       <c r="B96" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>12</v>
@@ -3270,7 +3276,7 @@
     </row>
     <row r="97" spans="1:7">
       <c r="B97" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>12</v>
@@ -3287,7 +3293,7 @@
     </row>
     <row r="98" spans="1:7">
       <c r="B98" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>12</v>
@@ -3324,7 +3330,7 @@
     </row>
     <row r="100" spans="1:7">
       <c r="B100" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>77</v>
@@ -3335,7 +3341,7 @@
     </row>
     <row r="101" spans="1:7">
       <c r="B101" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>77</v>
@@ -3346,7 +3352,7 @@
     </row>
     <row r="102" spans="1:7">
       <c r="B102" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>77</v>
@@ -3357,7 +3363,7 @@
     </row>
     <row r="103" spans="1:7">
       <c r="B103" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>77</v>
@@ -3368,7 +3374,7 @@
     </row>
     <row r="104" spans="1:7">
       <c r="B104" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>77</v>
@@ -3379,7 +3385,7 @@
     </row>
     <row r="105" spans="1:7">
       <c r="B105" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>77</v>
@@ -3390,7 +3396,7 @@
     </row>
     <row r="106" spans="1:7">
       <c r="B106" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>77</v>
@@ -3401,7 +3407,7 @@
     </row>
     <row r="107" spans="1:7">
       <c r="B107" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>77</v>
@@ -3412,13 +3418,13 @@
     </row>
     <row r="108" spans="1:7" ht="30">
       <c r="B108" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E108" s="1">
         <v>1</v>
@@ -3452,10 +3458,10 @@
     </row>
     <row r="110" spans="1:7">
       <c r="A110" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>12</v>
@@ -3472,10 +3478,10 @@
     </row>
     <row r="111" spans="1:7">
       <c r="A111" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>52</v>
@@ -3490,7 +3496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -3590,7 +3596,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="B5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -3663,7 +3669,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="B10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C10" t="s">
         <v>52</v>
@@ -3671,7 +3677,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="B11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C11" t="s">
         <v>52</v>
@@ -3805,7 +3811,7 @@
     </row>
     <row r="5" spans="1:10" ht="60">
       <c r="B5" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
@@ -5250,7 +5256,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD35"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.140625" defaultRowHeight="15"/>
@@ -5436,7 +5442,7 @@
         <v>33</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -5447,7 +5453,7 @@
         <v>33</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30">
@@ -5503,7 +5509,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="B15" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>12</v>
@@ -5554,40 +5560,40 @@
     </row>
     <row r="18" spans="1:7" ht="30">
       <c r="B18" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30">
       <c r="B19" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30">
       <c r="B20" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30">
       <c r="B21" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>12</v>
@@ -5638,13 +5644,13 @@
     </row>
     <row r="24" spans="1:7">
       <c r="B24" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -5669,7 +5675,7 @@
     </row>
     <row r="26" spans="1:7" ht="30">
       <c r="B26" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>77</v>
@@ -5686,7 +5692,7 @@
     </row>
     <row r="27" spans="1:7" ht="30">
       <c r="B27" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>12</v>
@@ -5737,13 +5743,13 @@
     </row>
     <row r="30" spans="1:7">
       <c r="B30" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -5768,7 +5774,7 @@
     </row>
     <row r="32" spans="1:7" ht="30">
       <c r="B32" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>12</v>
@@ -5805,10 +5811,10 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>12</v>
@@ -5825,10 +5831,10 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>52</v>
@@ -5842,10 +5848,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40:J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.42578125" defaultRowHeight="15"/>
@@ -5853,7 +5859,7 @@
     <col min="2" max="2" width="47.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1">
+    <row r="1" spans="1:10" s="5" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -5881,8 +5887,11 @@
       <c r="I1" s="5" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="6" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -5904,7 +5913,7 @@
       </c>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
@@ -5926,7 +5935,7 @@
       </c>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
@@ -5948,7 +5957,7 @@
       </c>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
@@ -5972,7 +5981,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="10" t="s">
         <v>132</v>
       </c>
@@ -5991,7 +6000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" s="10" t="s">
         <v>130</v>
       </c>
@@ -6002,7 +6011,7 @@
         <v>128</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10">
@@ -6012,7 +6021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -6034,7 +6043,7 @@
       </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -6056,7 +6065,7 @@
       </c>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
@@ -6078,7 +6087,7 @@
       </c>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -6102,7 +6111,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="A12" s="10" t="s">
         <v>132</v>
       </c>
@@ -6121,7 +6130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10">
       <c r="A13" s="10" t="s">
         <v>130</v>
       </c>
@@ -6142,7 +6151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
@@ -6164,7 +6173,7 @@
       </c>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
@@ -6186,7 +6195,7 @@
       </c>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10">
       <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
@@ -6554,7 +6563,7 @@
       </c>
       <c r="H32" s="5"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:10">
       <c r="A33" s="5" t="s">
         <v>13</v>
       </c>
@@ -6576,7 +6585,7 @@
       </c>
       <c r="H33" s="5"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:10">
       <c r="A34" s="5" t="s">
         <v>15</v>
       </c>
@@ -6598,7 +6607,7 @@
       </c>
       <c r="H34" s="5"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:10">
       <c r="A35" s="5" t="s">
         <v>15</v>
       </c>
@@ -6622,7 +6631,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:10">
       <c r="A36" s="10" t="s">
         <v>132</v>
       </c>
@@ -6641,7 +6650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:10">
       <c r="A37" s="10" t="s">
         <v>130</v>
       </c>
@@ -6652,7 +6661,7 @@
         <v>128</v>
       </c>
       <c r="D37" t="s">
-        <v>139</v>
+        <v>335</v>
       </c>
       <c r="E37" s="10"/>
       <c r="F37" s="10">
@@ -6662,7 +6671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:10">
       <c r="A38" s="5" t="s">
         <v>134</v>
       </c>
@@ -6684,7 +6693,7 @@
       </c>
       <c r="H38" s="5"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:10">
       <c r="A39" s="5" t="s">
         <v>13</v>
       </c>
@@ -6705,8 +6714,11 @@
         <v>2</v>
       </c>
       <c r="H39" s="5"/>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="J39" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" s="5" t="s">
         <v>15</v>
       </c>
@@ -6727,8 +6739,11 @@
         <v>3</v>
       </c>
       <c r="H40" s="5"/>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="J40" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" s="5" t="s">
         <v>15</v>
       </c>
@@ -6751,8 +6766,11 @@
       <c r="H41" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="J41" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" s="10" t="s">
         <v>132</v>
       </c>
@@ -6769,6 +6787,9 @@
       </c>
       <c r="G42" s="10">
         <v>1</v>
+      </c>
+      <c r="J42" t="s">
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -6891,10 +6912,10 @@
     </row>
     <row r="5" spans="1:10" ht="30">
       <c r="A5" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>12</v>
@@ -6928,13 +6949,13 @@
     </row>
     <row r="7" spans="1:10">
       <c r="B7" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E7" s="5">
         <v>1</v>
@@ -6948,13 +6969,13 @@
     </row>
     <row r="8" spans="1:10">
       <c r="B8" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G8" s="5">
         <v>3</v>
@@ -6962,7 +6983,7 @@
     </row>
     <row r="9" spans="1:10" ht="45">
       <c r="B9" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>12</v>
@@ -6979,7 +7000,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="B10" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>12</v>
@@ -6996,7 +7017,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="B11" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>12</v>
@@ -7013,7 +7034,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="B12" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>12</v>
@@ -7030,7 +7051,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="B13" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>52</v>
@@ -7157,7 +7178,7 @@
     </row>
     <row r="5" spans="1:10" ht="30">
       <c r="B5" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
@@ -7175,7 +7196,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="B6" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -7193,18 +7214,18 @@
     </row>
     <row r="7" spans="1:10">
       <c r="B7" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30">
       <c r="B8" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
@@ -7222,7 +7243,7 @@
     </row>
     <row r="9" spans="1:10" ht="45">
       <c r="B9" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>12</v>
@@ -7240,13 +7261,13 @@
     </row>
     <row r="10" spans="1:10">
       <c r="B10" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G10" s="1">
         <v>3</v>
@@ -7257,7 +7278,7 @@
         <v>101</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>12</v>
@@ -7275,7 +7296,7 @@
     </row>
     <row r="12" spans="1:10" ht="60">
       <c r="B12" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>12</v>
@@ -7293,7 +7314,7 @@
     </row>
     <row r="13" spans="1:10" ht="45">
       <c r="B13" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>12</v>
@@ -7311,7 +7332,7 @@
     </row>
     <row r="14" spans="1:10" ht="60">
       <c r="B14" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>12</v>
@@ -7329,7 +7350,7 @@
     </row>
     <row r="15" spans="1:10" ht="45">
       <c r="B15" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>12</v>
@@ -7347,7 +7368,7 @@
     </row>
     <row r="16" spans="1:10" ht="60">
       <c r="B16" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>12</v>
@@ -7365,7 +7386,7 @@
     </row>
     <row r="17" spans="1:7" ht="45">
       <c r="B17" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>12</v>
@@ -7383,7 +7404,7 @@
     </row>
     <row r="18" spans="1:7" ht="60">
       <c r="B18" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>12</v>
@@ -7401,7 +7422,7 @@
     </row>
     <row r="19" spans="1:7" ht="45">
       <c r="B19" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>12</v>
@@ -7419,7 +7440,7 @@
     </row>
     <row r="20" spans="1:7" ht="60">
       <c r="B20" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>12</v>
@@ -7437,7 +7458,7 @@
     </row>
     <row r="21" spans="1:7" ht="45">
       <c r="B21" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>12</v>
@@ -7455,10 +7476,10 @@
     </row>
     <row r="22" spans="1:7" ht="45">
       <c r="A22" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>12</v>
@@ -7476,7 +7497,7 @@
     </row>
     <row r="23" spans="1:7" ht="60">
       <c r="B23" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>12</v>
@@ -7494,7 +7515,7 @@
     </row>
     <row r="24" spans="1:7" ht="45">
       <c r="B24" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>12</v>
@@ -7512,7 +7533,7 @@
     </row>
     <row r="25" spans="1:7" ht="60">
       <c r="B25" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>12</v>
@@ -7530,7 +7551,7 @@
     </row>
     <row r="26" spans="1:7" ht="45">
       <c r="B26" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>12</v>
@@ -7548,7 +7569,7 @@
     </row>
     <row r="27" spans="1:7" ht="60">
       <c r="B27" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>12</v>
@@ -7566,7 +7587,7 @@
     </row>
     <row r="28" spans="1:7" ht="45">
       <c r="B28" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>12</v>
@@ -7584,7 +7605,7 @@
     </row>
     <row r="29" spans="1:7" ht="60">
       <c r="B29" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>12</v>
@@ -7602,7 +7623,7 @@
     </row>
     <row r="30" spans="1:7" ht="45">
       <c r="B30" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>12</v>
@@ -7620,7 +7641,7 @@
     </row>
     <row r="31" spans="1:7" ht="60">
       <c r="B31" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>12</v>
@@ -7638,7 +7659,7 @@
     </row>
     <row r="32" spans="1:7" ht="45">
       <c r="B32" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>12</v>
@@ -7656,10 +7677,10 @@
     </row>
     <row r="33" spans="1:7" ht="45">
       <c r="A33" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>12</v>
@@ -7677,7 +7698,7 @@
     </row>
     <row r="34" spans="1:7" ht="60">
       <c r="B34" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>12</v>
@@ -7695,7 +7716,7 @@
     </row>
     <row r="35" spans="1:7" ht="45">
       <c r="B35" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>12</v>
@@ -7713,7 +7734,7 @@
     </row>
     <row r="36" spans="1:7" ht="60">
       <c r="B36" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>12</v>
@@ -7731,7 +7752,7 @@
     </row>
     <row r="37" spans="1:7" ht="45">
       <c r="B37" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>12</v>
@@ -7749,7 +7770,7 @@
     </row>
     <row r="38" spans="1:7" ht="60">
       <c r="B38" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>12</v>
@@ -7767,7 +7788,7 @@
     </row>
     <row r="39" spans="1:7" ht="45">
       <c r="B39" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>12</v>
@@ -7785,7 +7806,7 @@
     </row>
     <row r="40" spans="1:7" ht="60">
       <c r="B40" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>12</v>
@@ -7803,7 +7824,7 @@
     </row>
     <row r="41" spans="1:7" ht="45">
       <c r="B41" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>12</v>
@@ -7821,10 +7842,10 @@
     </row>
     <row r="42" spans="1:7" ht="45">
       <c r="A42" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>12</v>
@@ -7842,7 +7863,7 @@
     </row>
     <row r="43" spans="1:7" ht="60">
       <c r="B43" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>12</v>
@@ -7860,7 +7881,7 @@
     </row>
     <row r="44" spans="1:7" ht="45">
       <c r="B44" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>12</v>
@@ -7878,7 +7899,7 @@
     </row>
     <row r="45" spans="1:7" ht="60">
       <c r="B45" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>12</v>
@@ -7896,7 +7917,7 @@
     </row>
     <row r="46" spans="1:7" ht="45">
       <c r="B46" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>12</v>
@@ -7914,7 +7935,7 @@
     </row>
     <row r="47" spans="1:7" ht="60">
       <c r="B47" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>12</v>
@@ -7932,7 +7953,7 @@
     </row>
     <row r="48" spans="1:7" ht="45">
       <c r="B48" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>12</v>
@@ -7950,10 +7971,10 @@
     </row>
     <row r="49" spans="1:7" ht="45">
       <c r="A49" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>12</v>
@@ -7971,7 +7992,7 @@
     </row>
     <row r="50" spans="1:7" ht="60">
       <c r="B50" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>12</v>
@@ -7989,10 +8010,10 @@
     </row>
     <row r="51" spans="1:7" ht="45">
       <c r="A51" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>12</v>
@@ -8010,7 +8031,7 @@
     </row>
     <row r="52" spans="1:7" ht="60">
       <c r="B52" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>12</v>
@@ -8028,10 +8049,10 @@
     </row>
     <row r="53" spans="1:7" ht="45">
       <c r="A53" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>12</v>
@@ -8049,7 +8070,7 @@
     </row>
     <row r="54" spans="1:7" ht="60">
       <c r="B54" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>12</v>
@@ -8067,10 +8088,10 @@
     </row>
     <row r="55" spans="1:7" ht="45">
       <c r="A55" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>12</v>
@@ -8088,7 +8109,7 @@
     </row>
     <row r="56" spans="1:7" ht="60">
       <c r="B56" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>12</v>
@@ -8106,10 +8127,10 @@
     </row>
     <row r="57" spans="1:7" ht="45">
       <c r="A57" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>12</v>
@@ -8127,7 +8148,7 @@
     </row>
     <row r="58" spans="1:7" ht="60">
       <c r="B58" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>12</v>
@@ -8145,10 +8166,10 @@
     </row>
     <row r="59" spans="1:7" ht="45">
       <c r="A59" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>12</v>
@@ -8166,7 +8187,7 @@
     </row>
     <row r="60" spans="1:7" ht="60">
       <c r="B60" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>12</v>
@@ -8184,10 +8205,10 @@
     </row>
     <row r="61" spans="1:7" ht="45">
       <c r="A61" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>12</v>
@@ -8205,7 +8226,7 @@
     </row>
     <row r="62" spans="1:7" ht="60">
       <c r="B62" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>12</v>
@@ -8223,10 +8244,10 @@
     </row>
     <row r="63" spans="1:7" ht="45">
       <c r="A63" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>12</v>
@@ -8244,7 +8265,7 @@
     </row>
     <row r="64" spans="1:7" ht="60">
       <c r="B64" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>12</v>
@@ -8262,10 +8283,10 @@
     </row>
     <row r="65" spans="1:7" ht="45">
       <c r="A65" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>12</v>
@@ -8283,7 +8304,7 @@
     </row>
     <row r="66" spans="1:7" ht="60">
       <c r="B66" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>12</v>
@@ -8301,10 +8322,10 @@
     </row>
     <row r="67" spans="1:7" ht="45">
       <c r="A67" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>12</v>
@@ -8322,7 +8343,7 @@
     </row>
     <row r="68" spans="1:7" ht="60">
       <c r="B68" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>12</v>
@@ -8340,10 +8361,10 @@
     </row>
     <row r="69" spans="1:7" ht="45">
       <c r="A69" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>12</v>
@@ -8361,7 +8382,7 @@
     </row>
     <row r="70" spans="1:7" ht="60">
       <c r="B70" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>12</v>
@@ -8379,10 +8400,10 @@
     </row>
     <row r="71" spans="1:7" ht="45">
       <c r="A71" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>12</v>
@@ -8400,7 +8421,7 @@
     </row>
     <row r="72" spans="1:7" ht="60">
       <c r="B72" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>12</v>
@@ -8418,10 +8439,10 @@
     </row>
     <row r="73" spans="1:7" ht="45">
       <c r="A73" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>12</v>
@@ -8439,7 +8460,7 @@
     </row>
     <row r="74" spans="1:7" ht="60">
       <c r="B74" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>12</v>
@@ -8457,10 +8478,10 @@
     </row>
     <row r="75" spans="1:7" ht="45">
       <c r="A75" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>12</v>
@@ -8478,7 +8499,7 @@
     </row>
     <row r="76" spans="1:7" ht="60">
       <c r="B76" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>12</v>
@@ -8496,10 +8517,10 @@
     </row>
     <row r="77" spans="1:7" ht="45">
       <c r="A77" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>12</v>
@@ -8517,7 +8538,7 @@
     </row>
     <row r="78" spans="1:7" ht="60">
       <c r="B78" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>12</v>
@@ -8535,10 +8556,10 @@
     </row>
     <row r="79" spans="1:7" ht="45">
       <c r="A79" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>12</v>
@@ -8556,7 +8577,7 @@
     </row>
     <row r="80" spans="1:7">
       <c r="B80" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>12</v>
@@ -8574,7 +8595,7 @@
     </row>
     <row r="81" spans="2:7" ht="45">
       <c r="B81" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C81" s="5" t="s">
         <v>12</v>
@@ -8592,7 +8613,7 @@
     </row>
     <row r="82" spans="2:7">
       <c r="B82" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>12</v>
@@ -8610,7 +8631,7 @@
     </row>
     <row r="83" spans="2:7">
       <c r="B83" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
fix for treatment planning
</commit_message>
<xml_diff>
--- a/resources/Clinician.xlsx
+++ b/resources/Clinician.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="17190" windowHeight="3345" tabRatio="736" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="17190" windowHeight="3345" tabRatio="736" firstSheet="18" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="Clinician" sheetId="1" r:id="rId1"/>
@@ -5314,18 +5314,6 @@
     <t>para</t>
   </si>
   <si>
-    <t>//textarea[@ng-model="vm.charts.dosage"]</t>
-  </si>
-  <si>
-    <t>//textarea[@ng-model="vm.charts.substance.doseName"]</t>
-  </si>
-  <si>
-    <t>//textarea[@ng-model="vm.charts.substance.routeName"]</t>
-  </si>
-  <si>
-    <t>//textarea[@ng-model="vm.charts.specialInstructions"]</t>
-  </si>
-  <si>
     <t>//input[@placeholder="Discontinue Date"]</t>
   </si>
   <si>
@@ -5381,6 +5369,18 @@
   </si>
   <si>
     <t>//p[@ng-if="vm.subtitle" and contains(text(),"TRAINING VISIT")]</t>
+  </si>
+  <si>
+    <t>//textarea[@ng-model="vm.medication.dosage"]</t>
+  </si>
+  <si>
+    <t>//textarea[@ng-model="vm.medication.substance.doseName"]</t>
+  </si>
+  <si>
+    <t>//textarea[@ng-model="vm.medication.substance.routeName"]</t>
+  </si>
+  <si>
+    <t>//textarea[@ng-model="vm.medication.specialInstructions"]</t>
   </si>
 </sst>
 </file>
@@ -32267,8 +32267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73:G73"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -33312,7 +33312,7 @@
     </row>
     <row r="54" spans="1:10">
       <c r="B54" s="1" t="s">
-        <v>1756</v>
+        <v>1775</v>
       </c>
       <c r="C54" t="s">
         <v>29</v>
@@ -33326,7 +33326,7 @@
     </row>
     <row r="55" spans="1:10">
       <c r="B55" s="1" t="s">
-        <v>1757</v>
+        <v>1776</v>
       </c>
       <c r="C55" t="s">
         <v>29</v>
@@ -33340,13 +33340,13 @@
     </row>
     <row r="56" spans="1:10">
       <c r="B56" s="1" t="s">
-        <v>1758</v>
+        <v>1777</v>
       </c>
       <c r="C56" t="s">
         <v>29</v>
       </c>
       <c r="D56" t="s">
-        <v>1761</v>
+        <v>1757</v>
       </c>
       <c r="J56" t="s">
         <v>1622</v>
@@ -33354,13 +33354,13 @@
     </row>
     <row r="57" spans="1:10">
       <c r="B57" s="1" t="s">
-        <v>1759</v>
+        <v>1778</v>
       </c>
       <c r="C57" t="s">
         <v>29</v>
       </c>
       <c r="D57" t="s">
-        <v>1762</v>
+        <v>1758</v>
       </c>
       <c r="J57" t="s">
         <v>1622</v>
@@ -33368,7 +33368,7 @@
     </row>
     <row r="58" spans="1:10">
       <c r="B58" s="1" t="s">
-        <v>1760</v>
+        <v>1756</v>
       </c>
       <c r="H58" t="s">
         <v>57</v>
@@ -33379,7 +33379,7 @@
     </row>
     <row r="59" spans="1:10">
       <c r="B59" s="1" t="s">
-        <v>1763</v>
+        <v>1759</v>
       </c>
       <c r="C59" t="s">
         <v>11</v>
@@ -33399,7 +33399,7 @@
     </row>
     <row r="60" spans="1:10">
       <c r="B60" s="1" t="s">
-        <v>1764</v>
+        <v>1760</v>
       </c>
       <c r="C60" t="s">
         <v>11</v>
@@ -33419,7 +33419,7 @@
     </row>
     <row r="61" spans="1:10" ht="30">
       <c r="B61" s="1" t="s">
-        <v>1765</v>
+        <v>1761</v>
       </c>
       <c r="C61" t="s">
         <v>11</v>
@@ -33439,7 +33439,7 @@
     </row>
     <row r="62" spans="1:10" ht="30">
       <c r="B62" s="1" t="s">
-        <v>1766</v>
+        <v>1762</v>
       </c>
       <c r="C62" t="s">
         <v>11</v>
@@ -33459,7 +33459,7 @@
     </row>
     <row r="63" spans="1:10" ht="30">
       <c r="B63" s="1" t="s">
-        <v>1767</v>
+        <v>1763</v>
       </c>
       <c r="C63" t="s">
         <v>11</v>
@@ -33502,7 +33502,7 @@
     </row>
     <row r="65" spans="1:10">
       <c r="B65" s="1" t="s">
-        <v>1770</v>
+        <v>1766</v>
       </c>
       <c r="C65" t="s">
         <v>11</v>
@@ -33545,7 +33545,7 @@
     </row>
     <row r="67" spans="1:10">
       <c r="B67" s="1" t="s">
-        <v>1771</v>
+        <v>1767</v>
       </c>
       <c r="C67" t="s">
         <v>11</v>
@@ -33588,7 +33588,7 @@
     </row>
     <row r="69" spans="1:10">
       <c r="B69" s="1" t="s">
-        <v>1772</v>
+        <v>1768</v>
       </c>
       <c r="C69" t="s">
         <v>11</v>
@@ -33631,7 +33631,7 @@
     </row>
     <row r="71" spans="1:10">
       <c r="B71" s="1" t="s">
-        <v>1773</v>
+        <v>1769</v>
       </c>
       <c r="C71" t="s">
         <v>11</v>
@@ -33674,7 +33674,7 @@
     </row>
     <row r="73" spans="1:10">
       <c r="B73" s="1" t="s">
-        <v>1774</v>
+        <v>1770</v>
       </c>
       <c r="C73" t="s">
         <v>11</v>
@@ -33717,7 +33717,7 @@
     </row>
     <row r="75" spans="1:10">
       <c r="B75" s="1" t="s">
-        <v>1775</v>
+        <v>1771</v>
       </c>
       <c r="C75" t="s">
         <v>11</v>
@@ -33737,7 +33737,7 @@
     </row>
     <row r="76" spans="1:10">
       <c r="B76" s="1" t="s">
-        <v>1776</v>
+        <v>1772</v>
       </c>
       <c r="C76" t="s">
         <v>11</v>
@@ -38451,7 +38451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -40822,13 +40822,13 @@
     </row>
     <row r="8" spans="1:10">
       <c r="B8" s="1" t="s">
-        <v>1768</v>
+        <v>1764</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>1777</v>
+        <v>1773</v>
       </c>
       <c r="E8" s="5">
         <v>1</v>
@@ -40865,7 +40865,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="B10" s="1" t="s">
-        <v>1769</v>
+        <v>1765</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>29</v>
@@ -40962,7 +40962,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="B15" s="1" t="s">
-        <v>1778</v>
+        <v>1774</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
fix comm notes and orders in clinician side
</commit_message>
<xml_diff>
--- a/resources/Clinician.xlsx
+++ b/resources/Clinician.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="17190" windowHeight="3345" tabRatio="736" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="17190" windowHeight="3345" tabRatio="736" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Clinician" sheetId="1" r:id="rId1"/>
@@ -5428,13 +5428,13 @@
     <t>//div[@class="_md-select-menu-container md-cs-content-theme-theme _md-active _md-clickable"]//md-option[6]</t>
   </si>
   <si>
-    <t>//p[contains(text(),"Physician Order")]</t>
-  </si>
-  <si>
     <t>Training Visit</t>
   </si>
   <si>
     <t>//p[@class="md-subhead md-card-head padding-0 ng-scope ng-binding" and contains(text(),"Training Visit")]</t>
+  </si>
+  <si>
+    <t>//p[contains(text(),"Exception Order")]</t>
   </si>
 </sst>
 </file>
@@ -39691,7 +39691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
@@ -40766,7 +40766,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40934,7 +40934,7 @@
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="E7" s="5">
         <v>1</v>
@@ -41068,7 +41068,7 @@
     </row>
     <row r="14" spans="1:10" ht="30">
       <c r="B14" s="1" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>45</v>
@@ -41087,8 +41087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15"/>
@@ -41350,7 +41350,7 @@
     </row>
     <row r="12" spans="1:10" ht="30">
       <c r="B12" s="1" t="s">
-        <v>1794</v>
+        <v>1796</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>45</v>

</xml_diff>